<commit_message>
Se actualiza los datos de pagos
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/Pagos/Pago_de_cuotas_data.xlsx
+++ b/src/test/resources/datadriven/Pagos/Pago_de_cuotas_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chm3572/Documents/GitHub/canalApp-auto-mobile-test-scp/src/test/resources/datadriven/Pagos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chm3572/GitChc/canalApp-auto-mobile-test-scp/src/test/resources/datadriven/Pagos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F3E038-9E5D-AE40-88B0-318D5A105500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143092A7-D26E-9946-91AB-BF10DC6FC843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29000" windowHeight="18880" xr2:uid="{01A04042-4CD8-B543-9BD3-9CD3C35333D1}"/>
+    <workbookView xWindow="4280" yWindow="760" windowWidth="24720" windowHeight="18880" activeTab="4" xr2:uid="{01A04042-4CD8-B543-9BD3-9CD3C35333D1}"/>
   </bookViews>
   <sheets>
     <sheet name="PagoSinTarjetaAsociada" sheetId="1" r:id="rId1"/>
@@ -95,13 +95,13 @@
     <t>El estado de cuenta está disponible para el contratante del seguro. Consulta con esa persona o empresa el estado de los pagos.</t>
   </si>
   <si>
-    <t>40975127</t>
-  </si>
-  <si>
-    <t>C3O-546</t>
-  </si>
-  <si>
-    <t>04/09/2025</t>
+    <t>72934725</t>
+  </si>
+  <si>
+    <t>XFN-363</t>
+  </si>
+  <si>
+    <t>06/11/2025</t>
   </si>
 </sst>
 </file>
@@ -212,150 +212,6 @@
   </cellStyles>
   <dxfs count="50">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -372,6 +228,260 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -426,20 +536,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -480,24 +576,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -552,20 +630,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -606,24 +670,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -678,98 +724,52 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica Neue"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -944,66 +944,66 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CB04384-F3AB-294E-8286-C30E57B12CA6}" name="Tabla33" displayName="Tabla33" ref="A1:G2" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EA995A8C-3F53-5E4A-964F-4316DFD118AE}" name="numeroUsuario" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{5C4447FE-3623-2A4D-B6A6-195EAC01E582}" name="contrasena" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{EA995A8C-3F53-5E4A-964F-4316DFD118AE}" name="numeroUsuario" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5C4447FE-3623-2A4D-B6A6-195EAC01E582}" name="contrasena" dataDxfId="38"/>
     <tableColumn id="3" xr3:uid="{704C3087-16C7-DE45-8EDA-D7AE479BAB92}" name="placa"/>
     <tableColumn id="4" xr3:uid="{77178DEE-791C-E949-885B-645569306E2F}" name="numtarjeta"/>
     <tableColumn id="5" xr3:uid="{E89B9A93-8E68-5D43-9AA0-365C159DF678}" name="fecha"/>
     <tableColumn id="6" xr3:uid="{9F66845D-DC05-B342-B80B-63F7039D14D5}" name="cvv"/>
-    <tableColumn id="7" xr3:uid="{E1F4145A-1C95-CB4E-BF0C-61DF0767B9F2}" name="vigencia" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{E1F4145A-1C95-CB4E-BF0C-61DF0767B9F2}" name="vigencia" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4DF3222F-5C20-E942-AD92-733D2E9AD974}" name="Tabla35" displayName="Tabla35" ref="A1:G2" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4DF3222F-5C20-E942-AD92-733D2E9AD974}" name="Tabla35" displayName="Tabla35" ref="A1:G2" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BA212CE2-9FDE-E541-81A0-CB547E72DEF1}" name="numeroUsuario" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{D310E9A4-DAC2-7B4B-A8A9-8286D0EB3B2D}" name="contrasena" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{98C221C3-8663-754A-A6B2-73E9C56D087D}" name="placa" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{BA212CE2-9FDE-E541-81A0-CB547E72DEF1}" name="numeroUsuario" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D310E9A4-DAC2-7B4B-A8A9-8286D0EB3B2D}" name="contrasena" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{98C221C3-8663-754A-A6B2-73E9C56D087D}" name="placa" dataDxfId="32"/>
     <tableColumn id="4" xr3:uid="{88BFEEA7-7E01-654F-BF19-36DCB6CEB1B7}" name="numtarjeta"/>
     <tableColumn id="5" xr3:uid="{DB4CF344-2832-5A4A-BA2A-2BC2FEDE6672}" name="fecha"/>
     <tableColumn id="6" xr3:uid="{0FA56893-0FCA-8E40-97DC-5A2AD2AA13B2}" name="cvv"/>
-    <tableColumn id="7" xr3:uid="{A3CA9F5E-1150-6D45-86F5-65FE77140D48}" name="vigencia" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{A3CA9F5E-1150-6D45-86F5-65FE77140D48}" name="vigencia" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F898A8F5-E726-9A45-B316-78D24CA1E6AE}" name="Tabla36" displayName="Tabla36" ref="A1:E2" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F898A8F5-E726-9A45-B316-78D24CA1E6AE}" name="Tabla36" displayName="Tabla36" ref="A1:E2" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{241E7033-85B6-5C4C-A37C-9DFC2E9F050A}" name="numeroUsuario" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{F5F8B8C0-406D-2344-8AAE-3274FDDF6874}" name="contrasena" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{F8562F7D-2330-7446-AE59-8E9814414317}" name="placa" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{241E7033-85B6-5C4C-A37C-9DFC2E9F050A}" name="numeroUsuario" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F5F8B8C0-406D-2344-8AAE-3274FDDF6874}" name="contrasena" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{F8562F7D-2330-7446-AE59-8E9814414317}" name="placa" dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{FA766CA1-FE87-4E41-AC5A-0BE3B0D9219A}" name="numtarjeta"/>
-    <tableColumn id="5" xr3:uid="{0352EE95-B00F-F44C-A56F-4C7E6E4C4CC1}" name="vigencia" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{0352EE95-B00F-F44C-A56F-4C7E6E4C4CC1}" name="vigencia" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{30706DF0-B237-9C4E-90D8-41493BEE640D}" name="Tabla37" displayName="Tabla37" ref="A1:G2" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{30706DF0-B237-9C4E-90D8-41493BEE640D}" name="Tabla37" displayName="Tabla37" ref="A1:G2" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{51AC6B01-55E7-4E42-92A1-E7BA57887FEF}" name="numeroUsuario" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{073D5C98-034A-2740-829B-73E8E48B5B7A}" name="contrasena" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F914BD94-03B2-294C-A63C-CA6EB99ADF59}" name="placa" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{51AC6B01-55E7-4E42-92A1-E7BA57887FEF}" name="numeroUsuario" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{073D5C98-034A-2740-829B-73E8E48B5B7A}" name="contrasena" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{F914BD94-03B2-294C-A63C-CA6EB99ADF59}" name="placa" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{1D456A14-3857-404A-801A-06C6A7BFE87E}" name="numtarjeta"/>
     <tableColumn id="5" xr3:uid="{E8381D8C-59D4-104E-BDFE-7E37684A9074}" name="fecha"/>
     <tableColumn id="6" xr3:uid="{EF2435E9-20B5-3A49-A351-72A60D74C8A1}" name="cvv"/>
-    <tableColumn id="7" xr3:uid="{B6E0D7A1-614E-864F-9B21-CA873486560E}" name="vigencia" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{B6E0D7A1-614E-864F-9B21-CA873486560E}" name="vigencia" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{86CF0329-2D74-5C42-830F-CC6195A0466C}" name="Tabla38" displayName="Tabla38" ref="A1:D2" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{86CF0329-2D74-5C42-830F-CC6195A0466C}" name="Tabla38" displayName="Tabla38" ref="A1:D2" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CAC6A610-B588-AF46-913B-520F35BB1BE6}" name="numeroUsuario" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{FB3CDD58-9AE1-E44F-8757-B10308FCBF0A}" name="contrasena" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{CAC6A610-B588-AF46-913B-520F35BB1BE6}" name="numeroUsuario" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{FB3CDD58-9AE1-E44F-8757-B10308FCBF0A}" name="contrasena" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{5654CDCE-3A4F-514E-BD77-C5D2F72B7733}" name="placa"/>
     <tableColumn id="4" xr3:uid="{077FBF02-5B0F-8B45-9B38-F65E3CF93192}" name="vigencia"/>
   </tableColumns>
@@ -1012,10 +1012,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{698D5E89-19DC-D345-B18D-4FBB30DEF5C1}" name="Tabla39" displayName="Tabla39" ref="A1:C2" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{698D5E89-19DC-D345-B18D-4FBB30DEF5C1}" name="Tabla39" displayName="Tabla39" ref="A1:C2" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0367689C-92AD-E445-AD4D-3E606BAE267A}" name="numeroUsuario" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{437B4A57-924C-F049-8615-5F39980F9FE4}" name="contrasena" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0367689C-92AD-E445-AD4D-3E606BAE267A}" name="numeroUsuario" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{437B4A57-924C-F049-8615-5F39980F9FE4}" name="contrasena" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{41A2D1A8-8CF2-7542-A292-74F660830C70}" name="mensaje"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1321,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82AA77F2-0857-FA48-A69B-EB35352C8AD3}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1592,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525B20BC-A25F-B542-8F2E-A481540F84F8}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se actualiza la data para pagos
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/Pagos/Pago_de_cuotas_data.xlsx
+++ b/src/test/resources/datadriven/Pagos/Pago_de_cuotas_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chm3572/GitChc/canalApp-auto-mobile-test-scp/src/test/resources/datadriven/Pagos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143092A7-D26E-9946-91AB-BF10DC6FC843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074FA9CF-6DD5-A14D-8F83-9C174D20ED90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="760" windowWidth="24720" windowHeight="18880" activeTab="4" xr2:uid="{01A04042-4CD8-B543-9BD3-9CD3C35333D1}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="21">
   <si>
     <t>numeroUsuario</t>
   </si>
@@ -98,10 +98,13 @@
     <t>72934725</t>
   </si>
   <si>
-    <t>XFN-363</t>
-  </si>
-  <si>
-    <t>06/11/2025</t>
+    <t>QLY-393</t>
+  </si>
+  <si>
+    <t>11/11/2025</t>
+  </si>
+  <si>
+    <t>XBV-171</t>
   </si>
 </sst>
 </file>
@@ -313,34 +316,6 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -536,6 +511,20 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -618,6 +607,20 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -944,7 +947,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CB04384-F3AB-294E-8286-C30E57B12CA6}" name="Tabla33" displayName="Tabla33" ref="A1:G2" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EA995A8C-3F53-5E4A-964F-4316DFD118AE}" name="numeroUsuario" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{EA995A8C-3F53-5E4A-964F-4316DFD118AE}" name="numeroUsuario" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{5C4447FE-3623-2A4D-B6A6-195EAC01E582}" name="contrasena" dataDxfId="38"/>
     <tableColumn id="3" xr3:uid="{704C3087-16C7-DE45-8EDA-D7AE479BAB92}" name="placa"/>
     <tableColumn id="4" xr3:uid="{77178DEE-791C-E949-885B-645569306E2F}" name="numtarjeta"/>
@@ -974,9 +977,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F898A8F5-E726-9A45-B316-78D24CA1E6AE}" name="Tabla36" displayName="Tabla36" ref="A1:E2" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{241E7033-85B6-5C4C-A37C-9DFC2E9F050A}" name="numeroUsuario" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F5F8B8C0-406D-2344-8AAE-3274FDDF6874}" name="contrasena" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{F8562F7D-2330-7446-AE59-8E9814414317}" name="placa" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{241E7033-85B6-5C4C-A37C-9DFC2E9F050A}" name="numeroUsuario" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{F5F8B8C0-406D-2344-8AAE-3274FDDF6874}" name="contrasena" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{F8562F7D-2330-7446-AE59-8E9814414317}" name="placa" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{FA766CA1-FE87-4E41-AC5A-0BE3B0D9219A}" name="numtarjeta"/>
     <tableColumn id="5" xr3:uid="{0352EE95-B00F-F44C-A56F-4C7E6E4C4CC1}" name="vigencia" dataDxfId="1"/>
   </tableColumns>
@@ -985,11 +988,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{30706DF0-B237-9C4E-90D8-41493BEE640D}" name="Tabla37" displayName="Tabla37" ref="A1:G2" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{30706DF0-B237-9C4E-90D8-41493BEE640D}" name="Tabla37" displayName="Tabla37" ref="A1:G2" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{51AC6B01-55E7-4E42-92A1-E7BA57887FEF}" name="numeroUsuario" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{073D5C98-034A-2740-829B-73E8E48B5B7A}" name="contrasena" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{F914BD94-03B2-294C-A63C-CA6EB99ADF59}" name="placa" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{51AC6B01-55E7-4E42-92A1-E7BA57887FEF}" name="numeroUsuario" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{073D5C98-034A-2740-829B-73E8E48B5B7A}" name="contrasena" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F914BD94-03B2-294C-A63C-CA6EB99ADF59}" name="placa" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{1D456A14-3857-404A-801A-06C6A7BFE87E}" name="numtarjeta"/>
     <tableColumn id="5" xr3:uid="{E8381D8C-59D4-104E-BDFE-7E37684A9074}" name="fecha"/>
     <tableColumn id="6" xr3:uid="{EF2435E9-20B5-3A49-A351-72A60D74C8A1}" name="cvv"/>
@@ -1000,10 +1003,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{86CF0329-2D74-5C42-830F-CC6195A0466C}" name="Tabla38" displayName="Tabla38" ref="A1:D2" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{86CF0329-2D74-5C42-830F-CC6195A0466C}" name="Tabla38" displayName="Tabla38" ref="A1:D2" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CAC6A610-B588-AF46-913B-520F35BB1BE6}" name="numeroUsuario" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{FB3CDD58-9AE1-E44F-8757-B10308FCBF0A}" name="contrasena" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{CAC6A610-B588-AF46-913B-520F35BB1BE6}" name="numeroUsuario" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{FB3CDD58-9AE1-E44F-8757-B10308FCBF0A}" name="contrasena" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{5654CDCE-3A4F-514E-BD77-C5D2F72B7733}" name="placa"/>
     <tableColumn id="4" xr3:uid="{077FBF02-5B0F-8B45-9B38-F65E3CF93192}" name="vigencia"/>
   </tableColumns>
@@ -1012,10 +1015,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{698D5E89-19DC-D345-B18D-4FBB30DEF5C1}" name="Tabla39" displayName="Tabla39" ref="A1:C2" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{698D5E89-19DC-D345-B18D-4FBB30DEF5C1}" name="Tabla39" displayName="Tabla39" ref="A1:C2" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0367689C-92AD-E445-AD4D-3E606BAE267A}" name="numeroUsuario" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{437B4A57-924C-F049-8615-5F39980F9FE4}" name="contrasena" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0367689C-92AD-E445-AD4D-3E606BAE267A}" name="numeroUsuario" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{437B4A57-924C-F049-8615-5F39980F9FE4}" name="contrasena" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{41A2D1A8-8CF2-7542-A292-74F660830C70}" name="mensaje"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1393,7 +1396,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>3</v>
@@ -1463,7 +1466,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>3</v>

</xml_diff>